<commit_message>
Updated code with new motor control process. Updated pinout documents to reflect changes.
</commit_message>
<xml_diff>
--- a/doc/MA_Pinout.xlsx
+++ b/doc/MA_Pinout.xlsx
@@ -136,21 +136,9 @@
     <t>ROptic</t>
   </si>
   <si>
-    <t>DrawRelay</t>
-  </si>
-  <si>
     <t>RGND</t>
   </si>
   <si>
-    <t>Interface relay signal governing draw state of winch.</t>
-  </si>
-  <si>
-    <t>RetractRelay</t>
-  </si>
-  <si>
-    <t>Interface relay signal governing retract state of winch.</t>
-  </si>
-  <si>
     <t>FireSolenoid</t>
   </si>
   <si>
@@ -188,13 +176,25 @@
   </si>
   <si>
     <t>LP:  Local power bus</t>
+  </si>
+  <si>
+    <t>motorEnable</t>
+  </si>
+  <si>
+    <t>motorDirection</t>
+  </si>
+  <si>
+    <t>Interface relay signal to enable or disable the motor.</t>
+  </si>
+  <si>
+    <t>Interface relay signal governing the direction the motor should move.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -204,22 +204,31 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,7 +239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -322,11 +331,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="8"/>
+      </left>
+      <right style="hair">
+        <color indexed="8"/>
+      </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -347,9 +372,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -651,7 +679,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -965,8 +993,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
+      <c r="A14" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
@@ -975,7 +1003,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="4">
         <v>0</v>
@@ -983,13 +1011,13 @@
       <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>42</v>
+      <c r="G14" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>43</v>
+      <c r="A15" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
@@ -998,7 +1026,7 @@
         <v>36</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="4">
         <v>0</v>
@@ -1006,13 +1034,13 @@
       <c r="F15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>44</v>
+      <c r="G15" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
@@ -1021,7 +1049,7 @@
         <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="4">
         <v>0</v>
@@ -1030,12 +1058,12 @@
         <v>18</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
@@ -1044,7 +1072,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>10</v>
@@ -1053,12 +1081,12 @@
         <v>18</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
@@ -1067,7 +1095,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>10</v>
@@ -1076,21 +1104,21 @@
         <v>18</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>10</v>
@@ -1099,7 +1127,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1113,17 +1141,17 @@
     </row>
     <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>